<commit_message>
Actualización de archivos REV-05-05-2025.xlsx y db.db con nuevos datos.
</commit_message>
<xml_diff>
--- a/REVs/REV-05-05-2025.xlsx
+++ b/REVs/REV-05-05-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2805,20 +2805,1054 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>4AF08793</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 62 BODY MIST 240 ML</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>4AF08794</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA SET BODY MIST</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>4AF08795</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 40 BODY MIST 90 ML</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>4AF08796</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 59 BODY MIST 90 ML</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>4AF08797</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 62 BODY MIST 90 ML</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>4AF08798</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 68 BODY MIST 90 ML</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>4AF08799</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO CHERIOSA 68 BODY MIST 240 ML</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>4AF08800</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>SOL DE JANEIRO RIO RADIANT BODY MIST 90 ML</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>6VA39715</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>WOOOW KIDNESS BRINGS HAPPINESS ESTUCHE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>1SH00472</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>GILLETTE KING C RECORTADORA BARBA STYLE MASTER</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>6VA37481</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>WOOOOW ESPEJO CUADRADO</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>6VA37480</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>WOOOOW CORTAUÑAS</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>6VA37482</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>WOOOOW CEPILLO PARA UÑAS</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>6VA38049</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>WOOOOW CEPILLO DOBLE CEJAS &amp; PESTAÑAS</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>6VA38050</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>WOOOOW PEINE METAL PESTAÑAS</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>6VA37479</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>WOOOOW CORTADOR CUTICULA</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>6VA24971</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ORAL B COMPLETE CEPILLO DENTAL 2UNDS</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>6VA37390</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>WOOOOW SET BROCHAS PEARL PINK</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>0TF27159</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>NIVEA Q10 FLUID SPF50 40ML</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>TRATAMIENTO CUERPO MANOS</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>0TF27157</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>LIPOSAN MANGO 4,8GR</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>TRATAMIENTO CUERPO MANOS</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>0TF27144</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SENCE LIP BALM ALOE VERA 2X4,3GRS</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>TRATAMIENTO CUERPO MANOS</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>8.6</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2BG03204</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>SENCE GLOW RODILLO FACIAL GIRLS</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BAÑO GEL</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Inject old revs files
</commit_message>
<xml_diff>
--- a/REVs/REV-05-05-2025.xlsx
+++ b/REVs/REV-05-05-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R72"/>
+  <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3839,20 +3839,114 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K72" t="inlineStr"/>
-      <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
-      <c r="N72" t="inlineStr"/>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr"/>
-      <c r="R72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2CA06708</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>REVLON COLORSTAY MASC.COLOR BOOSTER BLONDE 125ML</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>CABELLO ACONDIC. SUAVIZANTE</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2CN01618</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>CREME OF NATURE HONEY CREMA DEFINICION RIZOS 326GR</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>CABELLO TONICO LOCION</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>326</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
+      <c r="R74" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>